<commit_message>
upload of everything to date
</commit_message>
<xml_diff>
--- a/data/raw.data/Dire whelk.xlsx
+++ b/data/raw.data/Dire whelk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howardb\Documents\Academic Projects\Shellfish Mesocosms\Phase 1 - Feeding Trials\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howardb\Documents\Academic Projects\CFRA 2021 - Mesocosms\1_viu.feeding.trials\data\raw.data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -197,9 +197,6 @@
     <t>D-3</t>
   </si>
   <si>
-    <t>GRA-Lg6</t>
-  </si>
-  <si>
     <t>GRA-Lg25</t>
   </si>
   <si>
@@ -291,6 +288,9 @@
   </si>
   <si>
     <t>LV/AP</t>
+  </si>
+  <si>
+    <t>GRA-Lg06</t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2129,7 +2129,7 @@
         <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="F37">
         <v>2</v>
@@ -2170,7 +2170,7 @@
         <v>4</v>
       </c>
       <c r="E38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F38">
         <v>2</v>
@@ -2211,7 +2211,7 @@
         <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F39">
         <v>2</v>
@@ -2252,7 +2252,7 @@
         <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F40">
         <v>2</v>
@@ -2293,7 +2293,7 @@
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -2328,13 +2328,13 @@
         <v>48</v>
       </c>
       <c r="C42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
         <v>62</v>
-      </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>63</v>
       </c>
       <c r="F42">
         <v>2</v>
@@ -2360,7 +2360,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="M42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
@@ -2371,13 +2371,13 @@
         <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D43">
         <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F43">
         <v>2</v>
@@ -2403,7 +2403,7 @@
         <v>0</v>
       </c>
       <c r="M43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
@@ -2414,13 +2414,13 @@
         <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D44">
         <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F44">
         <v>2</v>
@@ -2446,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="M44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
@@ -2457,13 +2457,13 @@
         <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D45">
         <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F45">
         <v>2</v>
@@ -2489,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="M45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
@@ -2500,13 +2500,13 @@
         <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D46">
         <v>10</v>
       </c>
       <c r="E46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F46">
         <v>2</v>
@@ -2532,7 +2532,7 @@
         <v>0</v>
       </c>
       <c r="M46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
@@ -2543,13 +2543,13 @@
         <v>48</v>
       </c>
       <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
         <v>69</v>
-      </c>
-      <c r="D47">
-        <v>2</v>
-      </c>
-      <c r="E47" t="s">
-        <v>70</v>
       </c>
       <c r="F47">
         <v>2</v>
@@ -2575,7 +2575,7 @@
         <v>0</v>
       </c>
       <c r="M47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
@@ -2586,13 +2586,13 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D48">
         <v>4</v>
       </c>
       <c r="E48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F48">
         <v>2</v>
@@ -2618,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="M48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
@@ -2629,13 +2629,13 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D49">
         <v>6</v>
       </c>
       <c r="E49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F49">
         <v>2</v>
@@ -2661,7 +2661,7 @@
         <v>0</v>
       </c>
       <c r="M49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
@@ -2672,13 +2672,13 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D50">
         <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F50">
         <v>2</v>
@@ -2704,7 +2704,7 @@
         <v>0</v>
       </c>
       <c r="M50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
@@ -2715,7 +2715,7 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D51">
         <v>10</v>
@@ -2747,7 +2747,7 @@
         <v>0</v>
       </c>
       <c r="M51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
@@ -2758,13 +2758,13 @@
         <v>48</v>
       </c>
       <c r="C52" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
         <v>75</v>
-      </c>
-      <c r="D52">
-        <v>2</v>
-      </c>
-      <c r="E52" t="s">
-        <v>76</v>
       </c>
       <c r="F52">
         <v>3</v>
@@ -2790,7 +2790,7 @@
         <v>0</v>
       </c>
       <c r="M52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
@@ -2801,13 +2801,13 @@
         <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D53">
         <v>4</v>
       </c>
       <c r="E53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F53">
         <v>3</v>
@@ -2833,7 +2833,7 @@
         <v>0</v>
       </c>
       <c r="M53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
@@ -2844,13 +2844,13 @@
         <v>48</v>
       </c>
       <c r="C54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D54">
         <v>6</v>
       </c>
       <c r="E54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F54">
         <v>3</v>
@@ -2876,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="M54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
@@ -2887,13 +2887,13 @@
         <v>48</v>
       </c>
       <c r="C55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D55">
         <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F55">
         <v>3</v>
@@ -2919,7 +2919,7 @@
         <v>0</v>
       </c>
       <c r="M55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
@@ -2930,13 +2930,13 @@
         <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D56">
         <v>10</v>
       </c>
       <c r="E56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F56">
         <v>3</v>
@@ -2962,7 +2962,7 @@
         <v>0</v>
       </c>
       <c r="M56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
@@ -2973,13 +2973,13 @@
         <v>48</v>
       </c>
       <c r="C57" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
         <v>82</v>
-      </c>
-      <c r="D57">
-        <v>2</v>
-      </c>
-      <c r="E57" t="s">
-        <v>83</v>
       </c>
       <c r="F57">
         <v>2</v>
@@ -3005,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="M57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
@@ -3016,13 +3016,13 @@
         <v>48</v>
       </c>
       <c r="C58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D58">
         <v>4</v>
       </c>
       <c r="E58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F58">
         <v>2</v>
@@ -3048,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="M58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
@@ -3059,13 +3059,13 @@
         <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D59">
         <v>6</v>
       </c>
       <c r="E59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F59">
         <v>2</v>
@@ -3091,7 +3091,7 @@
         <v>3.6</v>
       </c>
       <c r="M59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
@@ -3102,13 +3102,13 @@
         <v>48</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D60">
         <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F60">
         <v>2</v>
@@ -3134,7 +3134,7 @@
         <v>2</v>
       </c>
       <c r="M60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
@@ -3145,13 +3145,13 @@
         <v>48</v>
       </c>
       <c r="C61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D61">
         <v>10</v>
       </c>
       <c r="E61" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F61">
         <v>2</v>
@@ -3177,7 +3177,7 @@
         <v>0</v>
       </c>
       <c r="M61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>